<commit_message>
FIX: programa funcionando interface nova e preenchendo todos os campos
</commit_message>
<xml_diff>
--- a/assets/modelo_declaracao.xlsx
+++ b/assets/modelo_declaracao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nataliel.vieira\Documents\NATALIEL 2\clone\teste\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F56E013-4B4A-4173-AA30-1D914307028E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859BD0C6-147F-4D82-BE71-9F61E3270CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5700" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -784,21 +784,165 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -814,150 +958,6 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13:Q13"/>
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1296,247 +1296,250 @@
     </row>
     <row r="2" spans="1:24" ht="8.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="75">
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="51">
         <f ca="1">NOW()</f>
-        <v>45623.725619444442</v>
-      </c>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="76"/>
+        <v>45624.366442361112</v>
+      </c>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="52"/>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="1"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="59"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="54"/>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="1"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="78" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="79" t="s">
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="48"/>
-      <c r="W4" s="48"/>
-      <c r="X4" s="59"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+      <c r="X4" s="54"/>
     </row>
     <row r="5" spans="1:24" ht="10.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="70" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="21"/>
-      <c r="V5" s="71"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="26"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="35"/>
     </row>
     <row r="6" spans="1:24" ht="9.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="70" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="21"/>
-      <c r="V6" s="71"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="26"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="35"/>
     </row>
     <row r="7" spans="1:24" ht="10.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="70" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="21"/>
-      <c r="V7" s="82"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="26"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="35"/>
     </row>
     <row r="8" spans="1:24" ht="9.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="70" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="84">
+      <c r="O8" s="32"/>
+      <c r="P8" s="44">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
-      </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="70" t="s">
+        <v>45624</v>
+      </c>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="U8" s="21"/>
-      <c r="V8" s="85"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="26"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="45">
+        <f ca="1">+NOW()</f>
+        <v>45624.366442361112</v>
+      </c>
+      <c r="W8" s="32"/>
+      <c r="X8" s="35"/>
     </row>
     <row r="9" spans="1:24" ht="12.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="88" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="36"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="88" t="s">
+      <c r="M9" s="21"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="41"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="27"/>
     </row>
     <row r="10" spans="1:24" ht="2.25" customHeight="1">
       <c r="A10" s="1"/>
@@ -1566,380 +1569,380 @@
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="92"/>
-      <c r="O11" s="92"/>
-      <c r="P11" s="92"/>
-      <c r="Q11" s="92"/>
-      <c r="R11" s="92"/>
-      <c r="S11" s="92"/>
-      <c r="T11" s="92"/>
-      <c r="U11" s="92"/>
-      <c r="V11" s="92"/>
-      <c r="W11" s="92"/>
-      <c r="X11" s="93"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="30"/>
     </row>
     <row r="12" spans="1:24" ht="9.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30" t="s">
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="30" t="s">
+      <c r="K12" s="88"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="31" t="s">
+      <c r="O12" s="88"/>
+      <c r="P12" s="88"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="28"/>
-      <c r="W12" s="28"/>
-      <c r="X12" s="32"/>
+      <c r="S12" s="88"/>
+      <c r="T12" s="88"/>
+      <c r="U12" s="88"/>
+      <c r="V12" s="88"/>
+      <c r="W12" s="88"/>
+      <c r="X12" s="92"/>
     </row>
     <row r="13" spans="1:24" ht="9.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="26"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="35"/>
     </row>
     <row r="14" spans="1:24" ht="9.75" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="26"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="35"/>
     </row>
     <row r="15" spans="1:24" ht="9.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="26"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="35"/>
     </row>
     <row r="16" spans="1:24" ht="9.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="26"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="35"/>
     </row>
     <row r="17" spans="1:26" ht="9.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="26"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="35"/>
     </row>
     <row r="18" spans="1:26" ht="9.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="26"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="35"/>
     </row>
     <row r="19" spans="1:26" ht="9.75" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="26"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="35"/>
     </row>
     <row r="20" spans="1:26" ht="9.75" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="26"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="35"/>
     </row>
     <row r="21" spans="1:26" ht="9.75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="26"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="35"/>
     </row>
     <row r="22" spans="1:26" ht="9.75" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="26"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="35"/>
       <c r="Z22" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="9.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="21"/>
-      <c r="P23" s="21"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="21"/>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="26"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="33"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="35"/>
     </row>
     <row r="24" spans="1:26" ht="9.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="40"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="36"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="41"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="72"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="73"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="27"/>
       <c r="Z24" s="6" t="s">
         <v>20</v>
       </c>
@@ -1972,97 +1975,97 @@
     </row>
     <row r="26" spans="1:26" ht="10.5" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="42" t="s">
+      <c r="J26" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="45" t="s">
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="45" t="s">
+      <c r="O26" s="75"/>
+      <c r="P26" s="75"/>
+      <c r="Q26" s="76"/>
+      <c r="R26" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="S26" s="43"/>
-      <c r="T26" s="43"/>
-      <c r="U26" s="43"/>
-      <c r="V26" s="43"/>
-      <c r="W26" s="43"/>
-      <c r="X26" s="46"/>
+      <c r="S26" s="75"/>
+      <c r="T26" s="75"/>
+      <c r="U26" s="75"/>
+      <c r="V26" s="75"/>
+      <c r="W26" s="75"/>
+      <c r="X26" s="78"/>
     </row>
     <row r="27" spans="1:26" ht="10.5" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="52" t="s">
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="53"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="51"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="50"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="54"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="84"/>
+      <c r="O27" s="81"/>
+      <c r="P27" s="81"/>
+      <c r="Q27" s="82"/>
+      <c r="R27" s="84"/>
+      <c r="S27" s="81"/>
+      <c r="T27" s="81"/>
+      <c r="U27" s="81"/>
+      <c r="V27" s="81"/>
+      <c r="W27" s="81"/>
+      <c r="X27" s="85"/>
     </row>
     <row r="28" spans="1:26" ht="10.5" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="56" t="s">
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="36"/>
-      <c r="W28" s="36"/>
-      <c r="X28" s="41"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="68"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="68"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="27"/>
     </row>
     <row r="29" spans="1:26" ht="4.5" customHeight="1">
       <c r="A29" s="1"/>
@@ -2095,107 +2098,107 @@
       <c r="B30" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C30" s="58" t="s">
+      <c r="C30" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
       <c r="I30" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="J30" s="58" t="s">
+      <c r="J30" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
       <c r="P30" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="Q30" s="58" t="s">
+      <c r="Q30" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="R30" s="48"/>
-      <c r="S30" s="48"/>
-      <c r="T30" s="48"/>
-      <c r="U30" s="48"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="59"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="49"/>
+      <c r="U30" s="49"/>
+      <c r="V30" s="49"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="54"/>
     </row>
     <row r="31" spans="1:26" ht="12" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C31" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
       <c r="I31" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="J31" s="58" t="s">
+      <c r="J31" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
       <c r="P31" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="Q31" s="58" t="s">
+      <c r="Q31" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="R31" s="48"/>
-      <c r="S31" s="48"/>
-      <c r="T31" s="48"/>
-      <c r="U31" s="48"/>
-      <c r="V31" s="48"/>
-      <c r="W31" s="48"/>
-      <c r="X31" s="59"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+      <c r="U31" s="49"/>
+      <c r="V31" s="49"/>
+      <c r="W31" s="49"/>
+      <c r="X31" s="54"/>
     </row>
     <row r="32" spans="1:26" ht="12" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C32" s="69" t="s">
+      <c r="C32" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I32" s="65"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="63"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="63"/>
-      <c r="U32" s="63"/>
-      <c r="V32" s="63"/>
-      <c r="W32" s="63"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="60"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="60"/>
+      <c r="T32" s="60"/>
+      <c r="U32" s="60"/>
+      <c r="V32" s="60"/>
+      <c r="W32" s="60"/>
       <c r="X32" s="13"/>
     </row>
     <row r="33" spans="2:24" ht="5.25" customHeight="1">
@@ -2203,56 +2206,56 @@
       <c r="X33" s="15"/>
     </row>
     <row r="34" spans="2:24" ht="15.75" customHeight="1">
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
-      <c r="P34" s="48"/>
-      <c r="Q34" s="48"/>
-      <c r="R34" s="48"/>
-      <c r="S34" s="48"/>
-      <c r="T34" s="48"/>
-      <c r="U34" s="48"/>
-      <c r="V34" s="48"/>
-      <c r="W34" s="48"/>
-      <c r="X34" s="59"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="49"/>
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="54"/>
     </row>
     <row r="35" spans="2:24" ht="9.75" customHeight="1">
-      <c r="B35" s="67"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="48"/>
-      <c r="R35" s="48"/>
-      <c r="S35" s="48"/>
-      <c r="T35" s="48"/>
-      <c r="U35" s="48"/>
-      <c r="V35" s="48"/>
-      <c r="W35" s="48"/>
-      <c r="X35" s="59"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="49"/>
+      <c r="U35" s="49"/>
+      <c r="V35" s="49"/>
+      <c r="W35" s="49"/>
+      <c r="X35" s="54"/>
     </row>
     <row r="36" spans="2:24" ht="7.5" customHeight="1">
       <c r="B36" s="14"/>
@@ -2260,87 +2263,87 @@
     </row>
     <row r="37" spans="2:24" ht="15.75" customHeight="1">
       <c r="B37" s="14"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="63"/>
-      <c r="L37" s="63"/>
-      <c r="M37" s="63"/>
-      <c r="N37" s="63"/>
-      <c r="O37" s="63"/>
-      <c r="P37" s="63"/>
-      <c r="R37" s="68"/>
-      <c r="S37" s="63"/>
-      <c r="T37" s="63"/>
-      <c r="U37" s="63"/>
-      <c r="V37" s="63"/>
-      <c r="W37" s="63"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="J37" s="64"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="R37" s="64"/>
+      <c r="S37" s="60"/>
+      <c r="T37" s="60"/>
+      <c r="U37" s="60"/>
+      <c r="V37" s="60"/>
+      <c r="W37" s="60"/>
       <c r="X37" s="15"/>
     </row>
     <row r="38" spans="2:24" ht="12" customHeight="1">
       <c r="B38" s="14"/>
-      <c r="C38" s="60" t="s">
+      <c r="C38" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="J38" s="60" t="s">
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="J38" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="48"/>
-      <c r="O38" s="48"/>
-      <c r="P38" s="48"/>
-      <c r="R38" s="60" t="s">
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="R38" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="S38" s="48"/>
-      <c r="T38" s="48"/>
-      <c r="U38" s="48"/>
-      <c r="V38" s="48"/>
-      <c r="W38" s="48"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="49"/>
+      <c r="U38" s="49"/>
+      <c r="V38" s="49"/>
+      <c r="W38" s="49"/>
       <c r="X38" s="15"/>
     </row>
     <row r="39" spans="2:24" ht="12" customHeight="1">
       <c r="B39" s="14"/>
-      <c r="C39" s="61" t="s">
+      <c r="C39" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="62"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="60"/>
       <c r="I39" s="16"/>
-      <c r="J39" s="61" t="s">
+      <c r="J39" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
-      <c r="M39" s="64">
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="61">
         <v>2381</v>
       </c>
-      <c r="N39" s="63"/>
-      <c r="O39" s="63"/>
-      <c r="P39" s="63"/>
+      <c r="N39" s="60"/>
+      <c r="O39" s="60"/>
+      <c r="P39" s="60"/>
       <c r="Q39" s="16"/>
-      <c r="R39" s="61" t="s">
+      <c r="R39" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="S39" s="48"/>
-      <c r="T39" s="62"/>
-      <c r="U39" s="63"/>
-      <c r="V39" s="63"/>
-      <c r="W39" s="63"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="59"/>
+      <c r="U39" s="60"/>
+      <c r="V39" s="60"/>
+      <c r="W39" s="60"/>
       <c r="X39" s="15"/>
     </row>
     <row r="40" spans="2:24" ht="15.75" customHeight="1">
@@ -3333,101 +3336,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="U9:X9"/>
-    <mergeCell ref="B11:X11"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:X15"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="E7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="V8:X8"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="B2:F4"/>
-    <mergeCell ref="G2:T3"/>
-    <mergeCell ref="U2:X4"/>
-    <mergeCell ref="G4:N4"/>
-    <mergeCell ref="O4:T4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:S5"/>
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M39:P39"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="T39:W39"/>
-    <mergeCell ref="I32:W32"/>
-    <mergeCell ref="B34:X35"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="J37:P37"/>
-    <mergeCell ref="R37:W37"/>
-    <mergeCell ref="J38:P38"/>
-    <mergeCell ref="R38:W38"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="R28:X28"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="J30:O30"/>
-    <mergeCell ref="Q30:X30"/>
-    <mergeCell ref="J31:O31"/>
-    <mergeCell ref="Q31:X31"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="R24:X24"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="R26:X26"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="R27:X27"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="R23:X23"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="R22:X22"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="R18:X18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="N21:Q21"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="R19:X19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="R20:X20"/>
-    <mergeCell ref="R21:X21"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="J16:M16"/>
     <mergeCell ref="N16:Q16"/>
@@ -3448,6 +3356,101 @@
     <mergeCell ref="J14:M14"/>
     <mergeCell ref="N14:Q14"/>
     <mergeCell ref="R14:X14"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="R18:X18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="R19:X19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="R20:X20"/>
+    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="R23:X23"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="R22:X22"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="R24:X24"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="R26:X26"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="R27:X27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="R28:X28"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="Q30:X30"/>
+    <mergeCell ref="J31:O31"/>
+    <mergeCell ref="Q31:X31"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M39:P39"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="T39:W39"/>
+    <mergeCell ref="I32:W32"/>
+    <mergeCell ref="B34:X35"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="J37:P37"/>
+    <mergeCell ref="R37:W37"/>
+    <mergeCell ref="J38:P38"/>
+    <mergeCell ref="R38:W38"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="B2:F4"/>
+    <mergeCell ref="G2:T3"/>
+    <mergeCell ref="U2:X4"/>
+    <mergeCell ref="G4:N4"/>
+    <mergeCell ref="O4:T4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:S5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="E7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="V8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="U9:X9"/>
+    <mergeCell ref="B11:X11"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="R15:X15"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="J15:M15"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D9" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>